<commit_message>
Adjusted RF circuit and layout
	- Removed mounting hole M3
	- Moved traces for button and led away
	- Clean up of the routing to have space for matching circuit on the bottom layer
	- Kept a clean solid GND on the layer directly below
	- Add shielding vias along the RF trace
</commit_message>
<xml_diff>
--- a/hw/wulpus_acquisition_pcb/docs/wulpus_acq_pcb_bom.xlsx
+++ b/hw/wulpus_acquisition_pcb/docs/wulpus_acq_pcb_bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s-fre\Github\wulpus\hw\wulpus_acquisition_pcb\Project Outputs for wulpus_acq_pcb\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s-fre\Github\wulpus\hw\wulpus_acquisition_pcb\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5725CFDE-9C18-4C26-BD22-4183962CDB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24B9A8F-F1A3-4D70-BA50-2382733CD962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{142B10BA-AE86-4987-BF36-3DAFB3C9F0E3}"/>
+    <workbookView xWindow="3390" yWindow="2925" windowWidth="21600" windowHeight="12645" xr2:uid="{EB7A9711-4281-4BB2-89FF-9AE7B0CFCA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="wulpus_acq_pcb_bom" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="146">
   <si>
     <t>Designator</t>
   </si>
@@ -141,7 +141,10 @@
     <t>E1</t>
   </si>
   <si>
-    <t>ANT-2.45-CHP-T</t>
+    <t>NN03-320</t>
+  </si>
+  <si>
+    <t>Fractus Antennas</t>
   </si>
   <si>
     <t>FB1, FB2, FB3</t>
@@ -219,6 +222,18 @@
     <t>742792040</t>
   </si>
   <si>
+    <t>L12</t>
+  </si>
+  <si>
+    <t>LQW18AN4N3G80D</t>
+  </si>
+  <si>
+    <t>L13</t>
+  </si>
+  <si>
+    <t>LQW15AN3N3G80D</t>
+  </si>
+  <si>
     <t>P1, P2</t>
   </si>
   <si>
@@ -303,49 +318,49 @@
     <t>CSRF0402FT10L0</t>
   </si>
   <si>
-    <t>R22, R35</t>
+    <t>R23, R27</t>
+  </si>
+  <si>
+    <t>CPF0402B324RE1</t>
+  </si>
+  <si>
+    <t>TE Connectivity / AMP</t>
+  </si>
+  <si>
+    <t>R24, R25</t>
+  </si>
+  <si>
+    <t>CRCW04021M00FKED</t>
+  </si>
+  <si>
+    <t>R26, R28</t>
+  </si>
+  <si>
+    <t>RC0402JR-0722RL</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>CRCW040247K0FKED</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>RC0603FR-07806RL</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>RC0603FR-071K82L</t>
+  </si>
+  <si>
+    <t>R35, R39</t>
   </si>
   <si>
     <t>CR0402-J/-000GLF</t>
-  </si>
-  <si>
-    <t>R23, R27</t>
-  </si>
-  <si>
-    <t>CPF0402B324RE1</t>
-  </si>
-  <si>
-    <t>TE Connectivity / AMP</t>
-  </si>
-  <si>
-    <t>R24, R25</t>
-  </si>
-  <si>
-    <t>CRCW04021M00FKED</t>
-  </si>
-  <si>
-    <t>R26, R28</t>
-  </si>
-  <si>
-    <t>RC0402JR-0722RL</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>CRCW040247K0FKED</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>RC0603FR-07806RL</t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
-    <t>RC0603FR-071K82L</t>
   </si>
   <si>
     <t>R36</t>
@@ -516,12 +531,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,14 +853,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A83F0C-162F-4A5C-88DA-8FAC4014C73D}">
-  <dimension ref="A1:D60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F733A09C-7F4B-4305-8D05-171A00CD5351}">
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -860,7 +883,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -874,7 +897,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -886,7 +909,7 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -900,7 +923,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -913,8 +936,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -928,7 +951,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -939,8 +962,8 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -952,7 +975,7 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -963,8 +986,8 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -976,7 +999,7 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -988,7 +1011,7 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1000,7 +1023,7 @@
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1012,7 +1035,7 @@
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1024,7 +1047,7 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1036,7 +1059,7 @@
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1045,42 +1068,44 @@
       <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>35</v>
+      <c r="A17" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>38</v>
+      <c r="A18" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>41</v>
+      <c r="A19" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -1088,25 +1113,25 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>43</v>
+      <c r="A20" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>46</v>
+      <c r="A21" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -1114,39 +1139,39 @@
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>48</v>
+      <c r="A22" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>51</v>
+      <c r="A23" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>54</v>
+      <c r="A24" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -1154,25 +1179,25 @@
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>56</v>
+      <c r="A25" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>58</v>
+      <c r="A26" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C26" s="1">
         <v>4</v>
@@ -1180,21 +1205,19 @@
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>60</v>
+      <c r="A27" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C27" s="1">
-        <v>2</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1206,127 +1229,127 @@
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="1">
         <v>8</v>
       </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="1">
-        <v>3</v>
-      </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C32" s="1">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-      <c r="D34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="1">
-        <v>2</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C36" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C37" s="1">
-        <v>1</v>
-      </c>
-      <c r="D37" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1335,24 +1358,24 @@
       <c r="C38" s="1">
         <v>2</v>
       </c>
-      <c r="D38" s="1"/>
+      <c r="D38" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>90</v>
+      <c r="A39" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C39" s="1">
-        <v>2</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>92</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="5" t="s">
         <v>93</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1361,92 +1384,90 @@
       <c r="C40" s="1">
         <v>2</v>
       </c>
-      <c r="D40" s="1"/>
+      <c r="D40" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>95</v>
+      <c r="A41" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C41" s="1">
         <v>2</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>97</v>
+      <c r="A42" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C42" s="1">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>99</v>
+      <c r="A43" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>101</v>
+      <c r="A44" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>103</v>
+      <c r="A45" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>105</v>
+      <c r="A46" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C46" s="1">
         <v>2</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>107</v>
-      </c>
+      <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -1455,24 +1476,26 @@
       <c r="C47" s="1">
         <v>1</v>
       </c>
-      <c r="D47" s="1"/>
+      <c r="D47" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="5" t="s">
         <v>110</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C48" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="5" t="s">
         <v>113</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -1481,12 +1504,10 @@
       <c r="C49" s="1">
         <v>1</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -1496,25 +1517,25 @@
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C51" s="1">
-        <v>1</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -1523,10 +1544,12 @@
       <c r="C52" s="1">
         <v>1</v>
       </c>
-      <c r="D52" s="1"/>
+      <c r="D52" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -1535,38 +1558,36 @@
       <c r="C53" s="1">
         <v>1</v>
       </c>
-      <c r="D53" s="1"/>
+      <c r="D53" s="2" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>124</v>
+      <c r="A54" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C54" s="1">
         <v>1</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>126</v>
+      <c r="A55" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>128</v>
-      </c>
+      <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -1575,10 +1596,12 @@
       <c r="C56" s="1">
         <v>1</v>
       </c>
-      <c r="D56" s="1"/>
+      <c r="D56" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="5" t="s">
         <v>131</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -1587,24 +1610,24 @@
       <c r="C57" s="1">
         <v>1</v>
       </c>
-      <c r="D57" s="1"/>
+      <c r="D57" s="2" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>133</v>
+      <c r="A58" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C58" s="1">
         <v>1</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>135</v>
-      </c>
+      <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="5" t="s">
         <v>136</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -1613,21 +1636,47 @@
       <c r="C59" s="1">
         <v>1</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
-      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="D62" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Expanded interpin distance for U8 to 0.22 mm plus updated siklscreen
</commit_message>
<xml_diff>
--- a/hw/wulpus_acquisition_pcb/docs/wulpus_acq_pcb_bom.xlsx
+++ b/hw/wulpus_acquisition_pcb/docs/wulpus_acq_pcb_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s-fre\Github\wulpus\hw\wulpus_acquisition_pcb\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serge\Documents\repos\wulpus_dev\hw\wulpus_acquisition_pcb\Project Outputs for wulpus_acq_pcb\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24B9A8F-F1A3-4D70-BA50-2382733CD962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1422F671-2F73-4DAE-BA14-8C9690BD7061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="2925" windowWidth="21600" windowHeight="12645" xr2:uid="{EB7A9711-4281-4BB2-89FF-9AE7B0CFCA6B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4BD6DF1A-A24D-4371-AFBD-A506F918C432}"/>
   </bookViews>
   <sheets>
     <sheet name="wulpus_acq_pcb_bom" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -485,7 +487,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -531,15 +533,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,39 +567,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -652,7 +651,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -763,13 +762,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -778,6 +770,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -842,33 +841,48 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F733A09C-7F4B-4305-8D05-171A00CD5351}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1A31C0-4CC4-42CA-A22F-75D675897263}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -882,8 +896,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -896,8 +910,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -908,8 +922,8 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -922,8 +936,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -936,8 +950,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -950,8 +964,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -962,8 +976,8 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -974,8 +988,8 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -986,8 +1000,8 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -998,8 +1012,8 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1010,8 +1024,8 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1022,8 +1036,8 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1034,8 +1048,8 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1046,8 +1060,8 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1058,8 +1072,8 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1072,8 +1086,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1086,8 +1100,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1100,8 +1114,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1112,8 +1126,8 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1126,8 +1140,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1138,8 +1152,8 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1152,8 +1166,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1166,8 +1180,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1178,8 +1192,8 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1192,8 +1206,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1204,8 +1218,8 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1216,8 +1230,8 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1228,8 +1242,8 @@
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1242,8 +1256,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1254,8 +1268,8 @@
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1266,8 +1280,8 @@
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1278,8 +1292,8 @@
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1292,8 +1306,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1306,8 +1320,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1320,8 +1334,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1334,8 +1348,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1348,8 +1362,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1362,8 +1376,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1374,8 +1388,8 @@
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1388,8 +1402,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1400,8 +1414,8 @@
       </c>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1414,8 +1428,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -1426,8 +1440,8 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -1440,8 +1454,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1454,8 +1468,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -1466,8 +1480,8 @@
       </c>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -1480,8 +1494,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -1494,8 +1508,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -1506,8 +1520,8 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -1520,8 +1534,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -1534,8 +1548,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -1548,8 +1562,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -1562,8 +1576,8 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -1574,8 +1588,8 @@
       </c>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -1586,8 +1600,8 @@
       </c>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -1600,8 +1614,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -1614,8 +1628,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -1626,8 +1640,8 @@
       </c>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -1638,8 +1652,8 @@
       </c>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -1652,8 +1666,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -1666,8 +1680,8 @@
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -1680,6 +1694,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>